<commit_message>
modified index and resultats excel
</commit_message>
<xml_diff>
--- a/MLP evaluacions/ResultatsTot.xlsx
+++ b/MLP evaluacions/ResultatsTot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\TFG-Perceptro\MLP evaluacions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SERGI\Documents\Uni\4rt any\2n quatri\TFG Perceptro\MLP evaluacions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775F43F0-BA28-4CD6-B01E-10AE6684B5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54972CAD-B9B1-4324-BB1B-2E2EF57CDE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2B169910-58A8-4BFB-B9DA-A680D5EE7EC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2B169910-58A8-4BFB-B9DA-A680D5EE7EC3}"/>
   </bookViews>
   <sheets>
     <sheet name="codificació 1" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,11 +149,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -175,25 +173,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -242,6 +221,25 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -256,16 +254,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D4D4699-4D50-4BAA-BE48-8054FB4970AE}" name="Tabla1" displayName="Tabla1" ref="A1:D50" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D4D4699-4D50-4BAA-BE48-8054FB4970AE}" name="Tabla1" displayName="Tabla1" ref="A1:D50" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:D50" xr:uid="{7D4D4699-4D50-4BAA-BE48-8054FB4970AE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D50">
     <sortCondition descending="1" ref="D1:D50"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{27063B57-93CB-4B99-9035-E6A90169CD51}" name="Arquitectura de xarxa" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B678E68E-16E8-4A06-A3B8-F30B05A8984C}" name="Funció d'avaluació" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{CEB03140-4012-4BF0-BE2C-11D0B9300482}" name="Resultat entrenament" dataDxfId="6" dataCellStyle="Millares"/>
-    <tableColumn id="4" xr3:uid="{7A523B5A-E4C3-4CD6-8C09-ABA540E37BF5}" name="Resultat test" dataDxfId="5" dataCellStyle="Millares"/>
+    <tableColumn id="1" xr3:uid="{27063B57-93CB-4B99-9035-E6A90169CD51}" name="Arquitectura de xarxa" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B678E68E-16E8-4A06-A3B8-F30B05A8984C}" name="Funció d'avaluació" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{CEB03140-4012-4BF0-BE2C-11D0B9300482}" name="Resultat entrenament" dataDxfId="5" dataCellStyle="Millares"/>
+    <tableColumn id="4" xr3:uid="{7A523B5A-E4C3-4CD6-8C09-ABA540E37BF5}" name="Resultat test" dataDxfId="4" dataCellStyle="Millares"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -584,21 +582,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D921C1-294A-4F0F-AFA9-EEE00E2326CE}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -612,691 +610,689 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.91152799129485995</v>
       </c>
-      <c r="D2" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.91152602434158303</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>0.91152602434158303</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.85503399372100797</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="3">
+        <v>0.85503399372100797</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="4">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="3">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>0.68720901012420599</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>0.61648619174957198</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>0.59823650121688798</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <v>0.50721508264541604</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>0.57899552583694402</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="3">
         <v>0.48116481304168701</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>0.57789897918701105</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="3">
         <v>0.480214804410934</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>0.57776302099227905</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="3">
         <v>0.47674477100372298</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>0.57716101408004705</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>0.47654476761817899</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <v>0.57520699501037598</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="3">
         <v>0.47439473867416299</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>0.57572102546691895</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="3">
         <v>0.47381472587585399</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>0.570034980773925</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="3">
         <v>0.46799468994140597</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="3">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="3">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="3">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="3">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="3">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="3">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="3">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="3">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="3">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="3">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="3">
         <v>0.46253463625907898</v>
       </c>
     </row>
@@ -1315,18 +1311,18 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1340,689 +1336,689 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6">
-        <v>0.91153150796890203</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.89525896310806197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="4">
+        <v>0.91153150796890203</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.89525896310806197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>0.91078197956085205</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>0.89335894584655695</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>0.91076749563217096</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="4">
         <v>0.89332890510559004</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D24" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D25" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D26" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="6">
-        <v>0.85503500699996904</v>
-      </c>
-      <c r="D27" s="6">
-        <v>0.81479817628860396</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="4">
+        <v>0.85503500699996904</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.81479817628860396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="4">
         <v>0.85458397865295399</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>0.81373810768127397</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="4">
         <v>0.85455048084259</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>0.81366813182830799</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="4">
         <v>0.68783152103423995</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>0.61606615781784002</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="4">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="4">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="4">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="4">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="4">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="4">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="4">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="4">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="4">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="4">
         <v>0.68706601858139005</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="4">
         <v>0.61588615179061801</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="4">
         <v>0.60749000310897805</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="4">
         <v>0.52182519435882502</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="4">
         <v>0.57947951555251997</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="4">
         <v>0.481654822826385</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="4">
         <v>0.578691005706787</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="4">
         <v>0.48104479908943099</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="4">
         <v>0.57981997728347701</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="4">
         <v>0.480214804410934</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="4">
         <v>0.57709097862243597</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="4">
         <v>0.47928479313850397</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="4">
         <v>0.57710349559783902</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="4">
         <v>0.47635477781295699</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="4">
         <v>0.57558250427246005</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="4">
         <v>0.47549474239349299</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.56676197052001898</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.46253463625907898</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="6">
-        <v>0.56676197052001898</v>
-      </c>
-      <c r="D44" s="6">
-        <v>0.46253463625907898</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="4">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="4">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="4">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="4">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="4">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="4">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="6">
+        <v>14</v>
+      </c>
+      <c r="C48" s="4">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="4">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="4">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="4">
         <v>0.46253463625907898</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="4">
         <v>0.56676197052001898</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="4">
         <v>0.46253463625907898</v>
       </c>
     </row>

</xml_diff>